<commit_message>
Got textures onto the rocket fins
</commit_message>
<xml_diff>
--- a/Rocket Profile.xlsx
+++ b/Rocket Profile.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/9438/School/Fall2019/hw6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{C320322A-B23F-2E4A-BF54-3C61A33767BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2307AFEE-1133-FF45-87C5-97CE9F6E14FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3060" windowWidth="28040" windowHeight="17440" xr2:uid="{7FAC806E-2875-F740-8FFB-814D429C524E}"/>
+    <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{7FAC806E-2875-F740-8FFB-814D429C524E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="rocket" sheetId="1" r:id="rId1"/>
+    <sheet name="fin" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="tdist">Sheet1!$D$34</definedName>
+    <definedName name="tdist">rocket!$D$34</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,6 +26,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -173,7 +185,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$A$33</c:f>
+              <c:f>rocket!$A$1:$A$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="33"/>
@@ -281,7 +293,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$33</c:f>
+              <c:f>rocket!$B$1:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="33"/>
@@ -648,7 +660,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$33</c:f>
+              <c:f>rocket!$F$2:$F$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -928,6 +940,568 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fin!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>fin!$A$2:$A$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="44"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14.1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>14.2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14.3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>14.3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14.3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>14.3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>13.8</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>13.6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>13.3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>13.1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>12.8</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>12.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12.4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>11.6</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>11.3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>10.9</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>10.4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9.9</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>fin!$B$2:$B$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="44"/>
+                <c:pt idx="0">
+                  <c:v>17.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>10.3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>10.9</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>11.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-05D3-3142-9DCF-FA24E4326F3C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="861483584"/>
+        <c:axId val="861485264"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="861483584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="861485264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="861485264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="861483584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1008,6 +1582,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2021,6 +2635,522 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2115,6 +3245,58 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>692150</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FD46FAB-606A-2640-B1AF-DEA90569F5B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6061731D-004F-6341-88DB-4F268CA330ED}" name="Table2" displayName="Table2" ref="A1:B45" totalsRowShown="0">
+  <autoFilter ref="A1:B45" xr:uid="{9F35022A-B7CF-924C-AB0E-E591FAFC1AE2}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{398B9CD5-D717-FA40-A2E2-FBCAFA8E1D2B}" name="x"/>
+    <tableColumn id="2" xr3:uid="{8A802740-AAE9-CD40-A578-2B034BB76CE6}" name="y"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2416,7 +3598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F864FD86-2014-EE4E-BF6F-5CE9AD330958}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G33"/>
     </sheetView>
   </sheetViews>
@@ -2452,7 +3634,7 @@
         <v>1.1661903789690609</v>
       </c>
       <c r="F2" s="2">
-        <f>E2/tdist</f>
+        <f t="shared" ref="F2:F33" si="0">E2/tdist</f>
         <v>3.2158681355893851E-2</v>
       </c>
       <c r="G2" s="2">
@@ -2467,7 +3649,7 @@
         <v>30.6</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D33" si="0">SQRT(POWER(A3-A2,2)+POWER(B3-B2,2))</f>
+        <f t="shared" ref="D3:D33" si="1">SQRT(POWER(A3-A2,2)+POWER(B3-B2,2))</f>
         <v>1.280624847486568</v>
       </c>
       <c r="E3">
@@ -2475,7 +3657,7 @@
         <v>2.4468152264556289</v>
       </c>
       <c r="F3" s="2">
-        <f>E3/tdist</f>
+        <f t="shared" si="0"/>
         <v>6.7472989507850648E-2</v>
       </c>
       <c r="G3" s="2">
@@ -2490,7 +3672,7 @@
         <v>29.5</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5556349186104057</v>
       </c>
       <c r="E4">
@@ -2498,7 +3680,7 @@
         <v>4.0024501450660344</v>
       </c>
       <c r="F4" s="2">
-        <f>E4/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.11037093186432854</v>
       </c>
       <c r="G4" s="2">
@@ -2513,7 +3695,7 @@
         <v>28.4</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.4212670403551906</v>
       </c>
       <c r="E5">
@@ -2521,7 +3703,7 @@
         <v>5.4237171854212249</v>
       </c>
       <c r="F5" s="2">
-        <f>E5/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.14956356687202096</v>
       </c>
       <c r="G5" s="2">
@@ -2536,7 +3718,7 @@
         <v>27.3</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.4212670403551881</v>
       </c>
       <c r="E6">
@@ -2544,7 +3726,7 @@
         <v>6.8449842257764129</v>
       </c>
       <c r="F6" s="2">
-        <f>E6/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.18875620187971329</v>
       </c>
       <c r="G6" s="2">
@@ -2559,7 +3741,7 @@
         <v>26.1</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3892443989449796</v>
       </c>
       <c r="E7">
@@ -2567,7 +3749,7 @@
         <v>8.2342286247213927</v>
       </c>
       <c r="F7" s="2">
-        <f>E7/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.22706578559504692</v>
       </c>
       <c r="G7" s="2">
@@ -2582,7 +3764,7 @@
         <v>25</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2529964086141683</v>
       </c>
       <c r="E8">
@@ -2590,7 +3772,7 @@
         <v>9.4872250333355606</v>
       </c>
       <c r="F8" s="2">
-        <f>E8/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.26161821628850185</v>
       </c>
       <c r="G8" s="2">
@@ -2605,7 +3787,7 @@
         <v>24</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1180339887498949</v>
       </c>
       <c r="E9">
@@ -2613,7 +3795,7 @@
         <v>10.605259022085455</v>
       </c>
       <c r="F9" s="2">
-        <f>E9/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.29244894464783838</v>
       </c>
       <c r="G9" s="2">
@@ -2628,7 +3810,7 @@
         <v>23</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0770329614269007</v>
       </c>
       <c r="E10">
@@ -2636,7 +3818,7 @@
         <v>11.682291983512357</v>
       </c>
       <c r="F10" s="2">
-        <f>E10/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.32214903516559884</v>
       </c>
       <c r="G10" s="2">
@@ -2651,7 +3833,7 @@
         <v>22</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.077032961426901</v>
       </c>
       <c r="E11">
@@ -2659,7 +3841,7 @@
         <v>12.759324944939259</v>
       </c>
       <c r="F11" s="2">
-        <f>E11/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.35184912568335924</v>
       </c>
       <c r="G11" s="2">
@@ -2674,7 +3856,7 @@
         <v>21</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.077032961426901</v>
       </c>
       <c r="E12">
@@ -2682,7 +3864,7 @@
         <v>13.83635790636616</v>
       </c>
       <c r="F12" s="2">
-        <f>E12/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.38154921620111965</v>
       </c>
       <c r="G12" s="2">
@@ -2697,7 +3879,7 @@
         <v>20</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0440306508910548</v>
       </c>
       <c r="E13">
@@ -2705,7 +3887,7 @@
         <v>14.880388557257215</v>
       </c>
       <c r="F13" s="2">
-        <f>E13/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.4103392402257327</v>
       </c>
       <c r="G13" s="2">
@@ -2720,7 +3902,7 @@
         <v>19</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0440306508910553</v>
       </c>
       <c r="E14">
@@ -2728,7 +3910,7 @@
         <v>15.92441920814827</v>
       </c>
       <c r="F14" s="2">
-        <f>E14/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.43912926425034582</v>
       </c>
       <c r="G14" s="2">
@@ -2743,7 +3925,7 @@
         <v>18</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0198039027185568</v>
       </c>
       <c r="E15">
@@ -2751,7 +3933,7 @@
         <v>16.944223110866826</v>
       </c>
       <c r="F15" s="2">
-        <f>E15/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.46725121530092384</v>
       </c>
       <c r="G15" s="2">
@@ -2766,7 +3948,7 @@
         <v>16.899999999999999</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1101801655587273</v>
       </c>
       <c r="E16">
@@ -2774,7 +3956,7 @@
         <v>18.054403276425553</v>
       </c>
       <c r="F16" s="2">
-        <f>E16/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.49786536787470681</v>
       </c>
       <c r="G16" s="2">
@@ -2789,7 +3971,7 @@
         <v>16</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.90138781886599595</v>
       </c>
       <c r="E17">
@@ -2797,7 +3979,7 @@
         <v>18.955791095291548</v>
       </c>
       <c r="F17" s="2">
-        <f>E17/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.52272189573478167</v>
       </c>
       <c r="G17" s="2">
@@ -2812,7 +3994,7 @@
         <v>15</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E18">
@@ -2820,7 +4002,7 @@
         <v>19.955791095291548</v>
       </c>
       <c r="F18" s="2">
-        <f>E18/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.5502977374977045</v>
       </c>
       <c r="G18" s="2">
@@ -2835,7 +4017,7 @@
         <v>14</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E19">
@@ -2843,7 +4025,7 @@
         <v>20.955791095291548</v>
       </c>
       <c r="F19" s="2">
-        <f>E19/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.57787357926062732</v>
       </c>
       <c r="G19" s="2">
@@ -2858,7 +4040,7 @@
         <v>13</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E20">
@@ -2866,7 +4048,7 @@
         <v>21.955791095291548</v>
       </c>
       <c r="F20" s="2">
-        <f>E20/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.60544942102355015</v>
       </c>
       <c r="G20" s="2">
@@ -2881,7 +4063,7 @@
         <v>12</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0012492197250393</v>
       </c>
       <c r="E21">
@@ -2889,7 +4071,7 @@
         <v>22.957040315016588</v>
       </c>
       <c r="F21" s="2">
-        <f>E21/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.63305971107193781</v>
       </c>
       <c r="G21" s="2">
@@ -2904,7 +4086,7 @@
         <v>11</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0012492197250393</v>
       </c>
       <c r="E22">
@@ -2912,7 +4094,7 @@
         <v>23.958289534741628</v>
       </c>
       <c r="F22" s="2">
-        <f>E22/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.66067000112032548</v>
       </c>
       <c r="G22" s="2">
@@ -2927,7 +4109,7 @@
         <v>10</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0049875621120892</v>
       </c>
       <c r="E23">
@@ -2935,7 +4117,7 @@
         <v>24.963277096853716</v>
       </c>
       <c r="F23" s="2">
-        <f>E23/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.688383379106834</v>
       </c>
       <c r="G23" s="2">
@@ -2950,7 +4132,7 @@
         <v>9</v>
       </c>
       <c r="D24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0198039027185568</v>
       </c>
       <c r="E24">
@@ -2958,7 +4140,7 @@
         <v>25.983080999572273</v>
       </c>
       <c r="F24" s="2">
-        <f>E24/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.71650533015741213</v>
       </c>
       <c r="G24" s="2">
@@ -2973,7 +4155,7 @@
         <v>8</v>
       </c>
       <c r="D25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0440306508910553</v>
       </c>
       <c r="E25">
@@ -2981,7 +4163,7 @@
         <v>27.027111650463329</v>
       </c>
       <c r="F25" s="2">
-        <f>E25/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.74529535418202519</v>
       </c>
       <c r="G25" s="2">
@@ -2996,7 +4178,7 @@
         <v>7</v>
       </c>
       <c r="D26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0440306508910548</v>
       </c>
       <c r="E26">
@@ -3004,7 +4186,7 @@
         <v>28.071142301354385</v>
       </c>
       <c r="F26" s="2">
-        <f>E26/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.77408537820663836</v>
       </c>
       <c r="G26" s="2">
@@ -3019,7 +4201,7 @@
         <v>5.9</v>
       </c>
       <c r="D27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1704699910719623</v>
       </c>
       <c r="E27">
@@ -3027,7 +4209,7 @@
         <v>29.241612292426346</v>
       </c>
       <c r="F27" s="2">
-        <f>E27/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.80636207346868849</v>
       </c>
       <c r="G27" s="2">
@@ -3042,7 +4224,7 @@
         <v>5</v>
       </c>
       <c r="D28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.98488578017961093</v>
       </c>
       <c r="E28">
@@ -3050,7 +4232,7 @@
         <v>30.226498072605956</v>
       </c>
       <c r="F28" s="2">
-        <f>E28/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.83352112789747423</v>
       </c>
       <c r="G28" s="2">
@@ -3065,7 +4247,7 @@
         <v>4</v>
       </c>
       <c r="D29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1180339887498949</v>
       </c>
       <c r="E29">
@@ -3073,7 +4255,7 @@
         <v>31.344532061355849</v>
       </c>
       <c r="F29" s="2">
-        <f>E29/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.86435185625681077</v>
       </c>
       <c r="G29" s="2">
@@ -3088,7 +4270,7 @@
         <v>3</v>
       </c>
       <c r="D30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1180339887498949</v>
       </c>
       <c r="E30">
@@ -3096,7 +4278,7 @@
         <v>32.462566050105742</v>
       </c>
       <c r="F30" s="2">
-        <f>E30/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.89518258461614719</v>
       </c>
       <c r="G30" s="2">
@@ -3111,7 +4293,7 @@
         <v>2</v>
       </c>
       <c r="D31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.16619037896906</v>
       </c>
       <c r="E31">
@@ -3119,7 +4301,7 @@
         <v>33.628756429074805</v>
       </c>
       <c r="F31" s="2">
-        <f>E31/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.92734126597204114</v>
       </c>
       <c r="G31" s="2">
@@ -3134,7 +4316,7 @@
         <v>1</v>
       </c>
       <c r="D32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2206555615733703</v>
       </c>
       <c r="E32">
@@ -3142,7 +4324,7 @@
         <v>34.849411990648179</v>
       </c>
       <c r="F32" s="2">
-        <f>E32/tdist</f>
+        <f t="shared" si="0"/>
         <v>0.96100187058502018</v>
       </c>
       <c r="G32" s="2">
@@ -3157,7 +4339,7 @@
         <v>0</v>
       </c>
       <c r="D33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.4142135623730951</v>
       </c>
       <c r="E33">
@@ -3165,7 +4347,7 @@
         <v>36.263625553021271</v>
       </c>
       <c r="F33" s="2">
-        <f>E33/tdist</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G33" s="2">
@@ -3182,4 +4364,392 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B08D5B3E-B63F-9E43-82D0-039634D56404}">
+  <dimension ref="A1:D45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>17.100000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <f>MIN(Table2[])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>8.1</v>
+      </c>
+      <c r="B4">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <f>MAX(Table2[])</f>
+        <v>17.100000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="B5">
+        <v>16.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>10.9</v>
+      </c>
+      <c r="B7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>11.8</v>
+      </c>
+      <c r="B8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>12.1</v>
+      </c>
+      <c r="B9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>12.6</v>
+      </c>
+      <c r="B10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>12.9</v>
+      </c>
+      <c r="B11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>13.1</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>13.4</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13.6</v>
+      </c>
+      <c r="B14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>13.8</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>13.9</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>14.1</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>14.2</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>14.3</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>14.3</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>14.3</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>14.3</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>13.8</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>13.6</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>13.3</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>13.1</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>12.8</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>12.7</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>12.4</v>
+      </c>
+      <c r="B30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>12.1</v>
+      </c>
+      <c r="B31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>12</v>
+      </c>
+      <c r="B32">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>11.8</v>
+      </c>
+      <c r="B33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>11.6</v>
+      </c>
+      <c r="B34">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>11.3</v>
+      </c>
+      <c r="B35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>11.2</v>
+      </c>
+      <c r="B36">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>10.9</v>
+      </c>
+      <c r="B37">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>10.4</v>
+      </c>
+      <c r="B38">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>9.9</v>
+      </c>
+      <c r="B39">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="B40">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="B41">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>8</v>
+      </c>
+      <c r="B42">
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>7</v>
+      </c>
+      <c r="B43">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>6.6</v>
+      </c>
+      <c r="B44">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>6</v>
+      </c>
+      <c r="B45">
+        <v>11.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cleaned up the fin shape
</commit_message>
<xml_diff>
--- a/Rocket Profile.xlsx
+++ b/Rocket Profile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/9438/School/Fall2019/hw6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2307AFEE-1133-FF45-87C5-97CE9F6E14FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9BE876-3D84-1149-958E-3248AC590758}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{7FAC806E-2875-F740-8FFB-814D429C524E}"/>
   </bookViews>
@@ -17,6 +17,15 @@
     <sheet name="fin" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">fin!$A$2:$A$45</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">fin!$B$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">fin!$B$2:$B$45</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">fin!$A$2:$A$45</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">fin!$B$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">fin!$B$2:$B$45</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">fin!$A$2:$A$45</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">fin!$B$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">fin!$B$2:$B$45</definedName>
     <definedName name="tdist">rocket!$D$34</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -968,11 +977,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="70" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -1005,23 +1014,27 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
+            <a:ln w="28575">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="4"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -1054,7 +1067,7 @@
                   <c:v>11.8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.1</c:v>
+                  <c:v>12.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>12.6</c:v>
@@ -1108,19 +1121,19 @@
                   <c:v>13.3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>13.1</c:v>
+                  <c:v>13.05</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>12.8</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>12.7</c:v>
+                  <c:v>12.6</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>12.4</c:v>
+                  <c:v>12.35</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>12.1</c:v>
+                  <c:v>12.2</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>12</c:v>
@@ -1132,7 +1145,7 @@
                   <c:v>11.6</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>11.3</c:v>
+                  <c:v>11.4</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>11.2</c:v>
@@ -1150,13 +1163,13 @@
                   <c:v>9.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>8.8000000000000007</c:v>
+                  <c:v>8.6</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>7</c:v>
+                  <c:v>7.3</c:v>
                 </c:pt>
                 <c:pt idx="42">
                   <c:v>6.6</c:v>
@@ -1177,7 +1190,7 @@
                   <c:v>17.100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17</c:v>
+                  <c:v>17.100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>17</c:v>
@@ -1261,7 +1274,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7</c:v>
+                  <c:v>6.7</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>7.5</c:v>
@@ -1282,25 +1295,25 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>10.3</c:v>
+                  <c:v>10.4</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>10.7</c:v>
+                  <c:v>10.6</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>10.7</c:v>
+                  <c:v>10.8</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>10.8</c:v>
+                  <c:v>10.9</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>10.9</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>11</c:v>
+                  <c:v>11.1</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>11</c:v>
+                  <c:v>11.15</c:v>
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>11.2</c:v>
@@ -1337,7 +1350,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -1353,14 +1366,8 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1371,9 +1378,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1399,7 +1406,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -1415,14 +1422,8 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1433,9 +1434,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1470,12 +1471,25 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="43000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="dk1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -2655,56 +2669,33 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="244">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -2712,16 +2703,52 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="43000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2738,16 +2765,11 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -2756,39 +2778,50 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="20000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:dataPointLine>
@@ -2796,7 +2829,7 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
@@ -2804,14 +2837,18 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -2819,7 +2856,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2835,16 +2872,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -2868,14 +2904,13 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2887,14 +2922,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -2906,14 +2940,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:errorBar>
@@ -2924,12 +2957,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -2941,7 +2968,7 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -2960,7 +2987,7 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
@@ -2977,156 +3004,164 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="0" kern="1200" spc="70" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="63500" cap="rnd" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="50000"/>
             <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -3135,22 +3170,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -3160,12 +3184,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -3251,16 +3269,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>692150</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4371,7 +4389,7 @@
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A2" sqref="A2:B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4397,7 +4415,7 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>17</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="D3">
         <f>MIN(Table2[])</f>
@@ -4450,7 +4468,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>12.1</v>
+        <v>12.2</v>
       </c>
       <c r="B9">
         <v>14</v>
@@ -4594,7 +4612,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>13.1</v>
+        <v>13.05</v>
       </c>
       <c r="B27">
         <v>3</v>
@@ -4610,7 +4628,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>12.7</v>
+        <v>12.6</v>
       </c>
       <c r="B29">
         <v>5</v>
@@ -4618,7 +4636,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>12.4</v>
+        <v>12.35</v>
       </c>
       <c r="B30">
         <v>6</v>
@@ -4626,10 +4644,10 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>12.1</v>
+        <v>12.2</v>
       </c>
       <c r="B31">
-        <v>7</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -4658,7 +4676,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>11.3</v>
+        <v>11.4</v>
       </c>
       <c r="B35">
         <v>9</v>
@@ -4685,7 +4703,7 @@
         <v>10.4</v>
       </c>
       <c r="B38">
-        <v>10.3</v>
+        <v>10.4</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -4693,7 +4711,7 @@
         <v>9.9</v>
       </c>
       <c r="B39">
-        <v>10.7</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -4701,15 +4719,15 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="B40">
-        <v>10.7</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>8.8000000000000007</v>
+        <v>8.6</v>
       </c>
       <c r="B41">
-        <v>10.8</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -4717,15 +4735,15 @@
         <v>8</v>
       </c>
       <c r="B42">
-        <v>10.9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>7</v>
+        <v>7.3</v>
       </c>
       <c r="B43">
-        <v>11</v>
+        <v>11.1</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -4733,7 +4751,7 @@
         <v>6.6</v>
       </c>
       <c r="B44">
-        <v>11</v>
+        <v>11.15</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>